<commit_message>
4th day update database and designed login page( stylesheet.css)
</commit_message>
<xml_diff>
--- a/ToniProject.xlsx
+++ b/ToniProject.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ServLet\Desktop\GonzalesToniDemeneseHub\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ServLet\Desktop\dict-toniproject\GonzalesToniERPInvoisEvalv\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
-    <sheet name="datamapping" sheetId="3" r:id="rId1"/>
-    <sheet name="Details" sheetId="4" r:id="rId2"/>
-    <sheet name="Overview" sheetId="5" r:id="rId3"/>
-    <sheet name="Design" sheetId="2" r:id="rId4"/>
+    <sheet name="Schema" sheetId="6" r:id="rId1"/>
+    <sheet name="datamapping" sheetId="3" r:id="rId2"/>
+    <sheet name="Details" sheetId="4" r:id="rId3"/>
+    <sheet name="Overview" sheetId="5" r:id="rId4"/>
+    <sheet name="Design" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="214">
   <si>
     <t>VENDORID</t>
   </si>
@@ -525,12 +526,219 @@
   <si>
     <t>ERPInvoisEvalv</t>
   </si>
+  <si>
+    <t>Tables_in_invoicedb</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> payments            </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> purchaseorders      </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> useraccess          </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> vendorinvcapture    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> vendors             </t>
+  </si>
+  <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>Null</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>Extra</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>MUL</t>
+  </si>
+  <si>
+    <t>PRI</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>varchar</t>
+  </si>
+  <si>
+    <t>purchaseorders</t>
+  </si>
+  <si>
+    <t>useraccess</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>pw</t>
+  </si>
+  <si>
+    <t>access</t>
+  </si>
+  <si>
+    <t>invAmount</t>
+  </si>
+  <si>
+    <t>vendorinvoicecapture</t>
+  </si>
+  <si>
+    <t>*User Name</t>
+  </si>
+  <si>
+    <t>*Password</t>
+  </si>
+  <si>
+    <t>enter username</t>
+  </si>
+  <si>
+    <t>enter password</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Microsoft YaHei UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>ERP</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Microsoft YaHei UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>InvoisEvalv</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Microsoft YaHei UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>Login</t>
+    </r>
+  </si>
+  <si>
+    <t>//5497844651</t>
+  </si>
+  <si>
+    <t>//BOFAUS3N</t>
+  </si>
+  <si>
+    <t>//for Europe country</t>
+  </si>
+  <si>
+    <t>https://transferwise.com/gb/blog/bank-of-america-swift-code</t>
+  </si>
+  <si>
+    <t>A SWIFT code is actually a few different parts and consists of 8-11 characters:</t>
+  </si>
+  <si>
+    <t>AAAA - Bank Code</t>
+  </si>
+  <si>
+    <t>BB - Country Code</t>
+  </si>
+  <si>
+    <t>CC - Location Code</t>
+  </si>
+  <si>
+    <t>DDD - Optional Branch Code</t>
+  </si>
+  <si>
+    <t>Bank Of America, N.A., 222 Broadway, New York, Ny 10038, United States Of America</t>
+  </si>
+  <si>
+    <t>100 North Tryon Street, Charlotte, North Carolina 28255</t>
+  </si>
+  <si>
+    <t>other address</t>
+  </si>
+  <si>
+    <t>----------+------------------+---------------+-------------+-----------------+---------------+--------------+-----------+-------------------+------------------------------------+</t>
+  </si>
+  <si>
+    <t>| vendorId | paymentReference | paymentStatus | beneficiary | bankName        | accountNumber | accountType  | swiftCode | bankAddressNumber | remittanceAdd                      |</t>
+  </si>
+  <si>
+    <t>+----------+------------------+---------------+-------------+-----------------+---------------+--------------+-----------+-------------------+------------------------------------+</t>
+  </si>
+  <si>
+    <t>|    10001 |         10000001 | paid          | Atlassians  | bank of america |        261232 | savings acct | BOFAUS3N  |          26123289 | North Carolina 28255               |</t>
+  </si>
+  <si>
+    <t>|    10001 |         10000002 | paid          | Atlassians  | bank of america |        261232 | savings acct | BOFAUS3N  |          26123289 | North Carolina 28255               |</t>
+  </si>
+  <si>
+    <t>|    10002 |         10000003 | paid          | Deltek Inc. | bank of america |        265262 | savings acct | BOFAUS3N  |          26526288 | Ny 10038, United States Of America |</t>
+  </si>
+  <si>
+    <t>|    10003 |         10000004 | paid          | Dell Inc.   | bank of america |        267563 | savings acct | BOFAUS3N  |          26526288 | Ny 10038, United States Of America |</t>
+  </si>
+  <si>
+    <t>|    10003 |         10000005 | unpaid        | Dell Inc.   | bank of america |        267563 | savings acct | BOFAUS3N  |          26526288 | Ny 10038, United States Of America |</t>
+  </si>
+  <si>
+    <t>----------+------------+-------------+---------------------------------+------------+-------------+----------+-------+---------+</t>
+  </si>
+  <si>
+    <t>| vendorId | subsidiary | vendorName  | vendorAddress                   | taxidssn   | paymentType | currency | terms | taxable |</t>
+  </si>
+  <si>
+    <t>+----------+------------+-------------+---------------------------------+------------+-------------+----------+-------+---------+</t>
+  </si>
+  <si>
+    <t>|    10001 | us         | Atlassians  | San San Francisco, CA 94103     | 20-3345959 | ach         | usd      | N30   | Yes     |</t>
+  </si>
+  <si>
+    <t>|    10002 | us         | Deltek Inc. | 509 Olive Way Seattle, WA 98101 | 20-3365454 | ach         | usd      | N15   | Yes     |</t>
+  </si>
+  <si>
+    <t>|    10003 | us         | Dell Inc.   | Round Rock, TexasÔÇÄ, USA       | 20-3376464 | wire        | usd      | N45   | Yes     |</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -610,8 +818,65 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Microsoft YaHei UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Microsoft YaHei UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Microsoft YaHei UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF0070C0"/>
+      <name val="Microsoft YaHei UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Microsoft YaHei UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -654,8 +919,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -777,11 +1060,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -855,6 +1162,58 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -952,16 +1311,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>601980</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>22861</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>160020</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>137161</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>421538</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>22861</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>444398</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>137161</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -978,7 +1337,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4259580" y="6972301"/>
+          <a:off x="4389120" y="6720841"/>
           <a:ext cx="4696358" cy="2194560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -990,16 +1349,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>399528</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>160020</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>15968</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>457466</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>1218</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>571765</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>85038</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1008,16 +1367,15 @@
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
-      <xdr:blipFill>
+      <xdr:blipFill rotWithShape="1">
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
+        <a:srcRect l="-473" t="7342" r="473" b="1129"/>
+        <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2342628" y="1257300"/>
-          <a:ext cx="9659138" cy="4047438"/>
+          <a:off x="5609048" y="8953500"/>
+          <a:ext cx="7870997" cy="3018738"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1031,13 +1389,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>121920</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>146889</xdr:rowOff>
+      <xdr:rowOff>93549</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>234491</xdr:colOff>
+      <xdr:colOff>89711</xdr:colOff>
       <xdr:row>87</xdr:row>
-      <xdr:rowOff>147796</xdr:rowOff>
+      <xdr:rowOff>94456</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1054,8 +1412,161 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="121920" y="12948489"/>
+          <a:off x="121920" y="12895149"/>
           <a:ext cx="6780071" cy="3109867"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>205740</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1143000</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1722120" y="1165860"/>
+          <a:ext cx="937260" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="00B0F0"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent3">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Login</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>224525</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>22861</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>182880</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>3351</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="224525" y="3345181"/>
+          <a:ext cx="9750055" cy="1077770"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>4466</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>98574</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="5646420"/>
+          <a:ext cx="13453766" cy="2895114"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1330,10 +1841,1159 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B5:X42"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.21875" style="59" customWidth="1"/>
+    <col min="2" max="2" width="17" style="59" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.77734375" style="59" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.33203125" style="60" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.109375" style="60" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.88671875" style="60" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.77734375" style="59" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5" style="59" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.88671875" style="59" customWidth="1"/>
+    <col min="10" max="10" width="18.6640625" style="59" customWidth="1"/>
+    <col min="11" max="11" width="7.5546875" style="59" customWidth="1"/>
+    <col min="12" max="12" width="6.33203125" style="59" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.109375" style="59" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.6640625" style="59" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.77734375" style="59" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5" style="59" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.109375" style="59" customWidth="1"/>
+    <col min="18" max="18" width="18.33203125" style="59" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.21875" style="59" customWidth="1"/>
+    <col min="20" max="20" width="6.33203125" style="60" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5" style="60" customWidth="1"/>
+    <col min="22" max="22" width="5.88671875" style="59" customWidth="1"/>
+    <col min="23" max="23" width="6.77734375" style="59" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5" style="59" bestFit="1" customWidth="1"/>
+    <col min="25" max="16384" width="8.88671875" style="59"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B5" s="64" t="s">
+        <v>177</v>
+      </c>
+      <c r="C5" s="65"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="65"/>
+      <c r="H5" s="67"/>
+      <c r="J5" s="64" t="s">
+        <v>148</v>
+      </c>
+      <c r="K5" s="65"/>
+      <c r="L5" s="66"/>
+      <c r="M5" s="66"/>
+      <c r="N5" s="66"/>
+      <c r="O5" s="65"/>
+      <c r="P5" s="67"/>
+      <c r="R5" s="64" t="s">
+        <v>182</v>
+      </c>
+      <c r="S5" s="65"/>
+      <c r="T5" s="66"/>
+      <c r="U5" s="66"/>
+      <c r="V5" s="66"/>
+      <c r="W5" s="65"/>
+      <c r="X5" s="67"/>
+    </row>
+    <row r="6" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B6" s="58" t="s">
+        <v>164</v>
+      </c>
+      <c r="C6" s="58" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" s="58" t="s">
+        <v>170</v>
+      </c>
+      <c r="E6" s="58" t="s">
+        <v>165</v>
+      </c>
+      <c r="F6" s="58" t="s">
+        <v>166</v>
+      </c>
+      <c r="G6" s="68" t="s">
+        <v>167</v>
+      </c>
+      <c r="H6" s="69" t="s">
+        <v>168</v>
+      </c>
+      <c r="J6" s="58" t="s">
+        <v>164</v>
+      </c>
+      <c r="K6" s="58" t="s">
+        <v>102</v>
+      </c>
+      <c r="L6" s="58" t="s">
+        <v>170</v>
+      </c>
+      <c r="M6" s="58" t="s">
+        <v>165</v>
+      </c>
+      <c r="N6" s="58" t="s">
+        <v>166</v>
+      </c>
+      <c r="O6" s="68" t="s">
+        <v>167</v>
+      </c>
+      <c r="P6" s="69" t="s">
+        <v>168</v>
+      </c>
+      <c r="R6" s="58" t="s">
+        <v>164</v>
+      </c>
+      <c r="S6" s="58" t="s">
+        <v>102</v>
+      </c>
+      <c r="T6" s="58" t="s">
+        <v>170</v>
+      </c>
+      <c r="U6" s="58" t="s">
+        <v>165</v>
+      </c>
+      <c r="V6" s="58" t="s">
+        <v>166</v>
+      </c>
+      <c r="W6" s="68" t="s">
+        <v>167</v>
+      </c>
+      <c r="X6" s="69" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="7" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B7" s="70" t="s">
+        <v>178</v>
+      </c>
+      <c r="C7" s="70" t="s">
+        <v>175</v>
+      </c>
+      <c r="D7" s="71">
+        <v>15</v>
+      </c>
+      <c r="E7" s="71" t="s">
+        <v>171</v>
+      </c>
+      <c r="F7" s="71" t="s">
+        <v>173</v>
+      </c>
+      <c r="G7" s="70" t="s">
+        <v>174</v>
+      </c>
+      <c r="H7" s="72"/>
+      <c r="J7" s="70" t="s">
+        <v>115</v>
+      </c>
+      <c r="K7" s="70" t="s">
+        <v>169</v>
+      </c>
+      <c r="L7" s="71">
+        <v>5</v>
+      </c>
+      <c r="M7" s="71" t="s">
+        <v>171</v>
+      </c>
+      <c r="N7" s="71" t="s">
+        <v>172</v>
+      </c>
+      <c r="O7" s="70" t="s">
+        <v>174</v>
+      </c>
+      <c r="P7" s="72"/>
+      <c r="R7" s="70" t="s">
+        <v>130</v>
+      </c>
+      <c r="S7" s="70" t="s">
+        <v>175</v>
+      </c>
+      <c r="T7" s="71">
+        <v>25</v>
+      </c>
+      <c r="U7" s="71" t="s">
+        <v>171</v>
+      </c>
+      <c r="V7" s="71" t="s">
+        <v>173</v>
+      </c>
+      <c r="W7" s="70" t="s">
+        <v>174</v>
+      </c>
+      <c r="X7" s="70"/>
+    </row>
+    <row r="8" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B8" s="73" t="s">
+        <v>179</v>
+      </c>
+      <c r="C8" s="73" t="s">
+        <v>175</v>
+      </c>
+      <c r="D8" s="74">
+        <v>16</v>
+      </c>
+      <c r="E8" s="74" t="s">
+        <v>171</v>
+      </c>
+      <c r="F8" s="74"/>
+      <c r="G8" s="73" t="s">
+        <v>174</v>
+      </c>
+      <c r="H8" s="75"/>
+      <c r="J8" s="73" t="s">
+        <v>126</v>
+      </c>
+      <c r="K8" s="73" t="s">
+        <v>169</v>
+      </c>
+      <c r="L8" s="74">
+        <v>10</v>
+      </c>
+      <c r="M8" s="74" t="s">
+        <v>171</v>
+      </c>
+      <c r="N8" s="74" t="s">
+        <v>173</v>
+      </c>
+      <c r="O8" s="73" t="s">
+        <v>174</v>
+      </c>
+      <c r="P8" s="75"/>
+      <c r="R8" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="S8" s="73" t="s">
+        <v>169</v>
+      </c>
+      <c r="T8" s="74">
+        <v>8</v>
+      </c>
+      <c r="U8" s="74" t="s">
+        <v>171</v>
+      </c>
+      <c r="V8" s="74" t="s">
+        <v>172</v>
+      </c>
+      <c r="W8" s="73" t="s">
+        <v>174</v>
+      </c>
+      <c r="X8" s="73"/>
+    </row>
+    <row r="9" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B9" s="76" t="s">
+        <v>180</v>
+      </c>
+      <c r="C9" s="76" t="s">
+        <v>175</v>
+      </c>
+      <c r="D9" s="77">
+        <v>50</v>
+      </c>
+      <c r="E9" s="77" t="s">
+        <v>171</v>
+      </c>
+      <c r="F9" s="77"/>
+      <c r="G9" s="76" t="s">
+        <v>174</v>
+      </c>
+      <c r="H9" s="78"/>
+      <c r="J9" s="73" t="s">
+        <v>127</v>
+      </c>
+      <c r="K9" s="73" t="s">
+        <v>175</v>
+      </c>
+      <c r="L9" s="74">
+        <v>25</v>
+      </c>
+      <c r="M9" s="74" t="s">
+        <v>171</v>
+      </c>
+      <c r="N9" s="74"/>
+      <c r="O9" s="73" t="s">
+        <v>174</v>
+      </c>
+      <c r="P9" s="75"/>
+      <c r="R9" s="73" t="s">
+        <v>115</v>
+      </c>
+      <c r="S9" s="73" t="s">
+        <v>169</v>
+      </c>
+      <c r="T9" s="74">
+        <v>5</v>
+      </c>
+      <c r="U9" s="74" t="s">
+        <v>171</v>
+      </c>
+      <c r="V9" s="74" t="s">
+        <v>172</v>
+      </c>
+      <c r="W9" s="73" t="s">
+        <v>174</v>
+      </c>
+      <c r="X9" s="73"/>
+    </row>
+    <row r="10" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="J10" s="73" t="s">
+        <v>140</v>
+      </c>
+      <c r="K10" s="73" t="s">
+        <v>175</v>
+      </c>
+      <c r="L10" s="74">
+        <v>50</v>
+      </c>
+      <c r="M10" s="74" t="s">
+        <v>171</v>
+      </c>
+      <c r="N10" s="74"/>
+      <c r="O10" s="73" t="s">
+        <v>174</v>
+      </c>
+      <c r="P10" s="75"/>
+      <c r="R10" s="73" t="s">
+        <v>129</v>
+      </c>
+      <c r="S10" s="73" t="s">
+        <v>175</v>
+      </c>
+      <c r="T10" s="74">
+        <v>25</v>
+      </c>
+      <c r="U10" s="74" t="s">
+        <v>171</v>
+      </c>
+      <c r="V10" s="74"/>
+      <c r="W10" s="73" t="s">
+        <v>174</v>
+      </c>
+      <c r="X10" s="73"/>
+    </row>
+    <row r="11" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="J11" s="73" t="s">
+        <v>141</v>
+      </c>
+      <c r="K11" s="73" t="s">
+        <v>175</v>
+      </c>
+      <c r="L11" s="74">
+        <v>50</v>
+      </c>
+      <c r="M11" s="74" t="s">
+        <v>171</v>
+      </c>
+      <c r="N11" s="74"/>
+      <c r="O11" s="73" t="s">
+        <v>174</v>
+      </c>
+      <c r="P11" s="75"/>
+      <c r="R11" s="73" t="s">
+        <v>131</v>
+      </c>
+      <c r="S11" s="73" t="s">
+        <v>175</v>
+      </c>
+      <c r="T11" s="74">
+        <v>25</v>
+      </c>
+      <c r="U11" s="74" t="s">
+        <v>171</v>
+      </c>
+      <c r="V11" s="74"/>
+      <c r="W11" s="73" t="s">
+        <v>174</v>
+      </c>
+      <c r="X11" s="73"/>
+    </row>
+    <row r="12" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B12" s="58" t="s">
+        <v>158</v>
+      </c>
+      <c r="J12" s="73" t="s">
+        <v>152</v>
+      </c>
+      <c r="K12" s="73" t="s">
+        <v>169</v>
+      </c>
+      <c r="L12" s="74">
+        <v>11</v>
+      </c>
+      <c r="M12" s="74" t="s">
+        <v>171</v>
+      </c>
+      <c r="N12" s="74"/>
+      <c r="O12" s="73" t="s">
+        <v>174</v>
+      </c>
+      <c r="P12" s="75"/>
+      <c r="R12" s="73" t="s">
+        <v>132</v>
+      </c>
+      <c r="S12" s="73" t="s">
+        <v>175</v>
+      </c>
+      <c r="T12" s="74">
+        <v>5</v>
+      </c>
+      <c r="U12" s="74" t="s">
+        <v>171</v>
+      </c>
+      <c r="V12" s="74"/>
+      <c r="W12" s="73" t="s">
+        <v>174</v>
+      </c>
+      <c r="X12" s="73"/>
+    </row>
+    <row r="13" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B13" s="61" t="s">
+        <v>159</v>
+      </c>
+      <c r="J13" s="73" t="s">
+        <v>108</v>
+      </c>
+      <c r="K13" s="73" t="s">
+        <v>175</v>
+      </c>
+      <c r="L13" s="74">
+        <v>25</v>
+      </c>
+      <c r="M13" s="74" t="s">
+        <v>171</v>
+      </c>
+      <c r="N13" s="74"/>
+      <c r="O13" s="73" t="s">
+        <v>174</v>
+      </c>
+      <c r="P13" s="75"/>
+      <c r="R13" s="73" t="s">
+        <v>181</v>
+      </c>
+      <c r="S13" s="73" t="s">
+        <v>169</v>
+      </c>
+      <c r="T13" s="74">
+        <v>11</v>
+      </c>
+      <c r="U13" s="74" t="s">
+        <v>171</v>
+      </c>
+      <c r="V13" s="74"/>
+      <c r="W13" s="73" t="s">
+        <v>174</v>
+      </c>
+      <c r="X13" s="73"/>
+    </row>
+    <row r="14" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B14" s="62" t="s">
+        <v>160</v>
+      </c>
+      <c r="J14" s="73" t="s">
+        <v>143</v>
+      </c>
+      <c r="K14" s="73" t="s">
+        <v>175</v>
+      </c>
+      <c r="L14" s="74">
+        <v>50</v>
+      </c>
+      <c r="M14" s="74" t="s">
+        <v>171</v>
+      </c>
+      <c r="N14" s="74"/>
+      <c r="O14" s="73" t="s">
+        <v>174</v>
+      </c>
+      <c r="P14" s="75"/>
+      <c r="R14" s="73" t="s">
+        <v>133</v>
+      </c>
+      <c r="S14" s="73" t="s">
+        <v>169</v>
+      </c>
+      <c r="T14" s="74">
+        <v>11</v>
+      </c>
+      <c r="U14" s="74" t="s">
+        <v>171</v>
+      </c>
+      <c r="V14" s="74"/>
+      <c r="W14" s="73" t="s">
+        <v>174</v>
+      </c>
+      <c r="X14" s="73"/>
+    </row>
+    <row r="15" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B15" s="62" t="s">
+        <v>161</v>
+      </c>
+      <c r="J15" s="73" t="s">
+        <v>144</v>
+      </c>
+      <c r="K15" s="73" t="s">
+        <v>169</v>
+      </c>
+      <c r="L15" s="74">
+        <v>11</v>
+      </c>
+      <c r="M15" s="74" t="s">
+        <v>171</v>
+      </c>
+      <c r="N15" s="74"/>
+      <c r="O15" s="73" t="s">
+        <v>174</v>
+      </c>
+      <c r="P15" s="75"/>
+      <c r="R15" s="73" t="s">
+        <v>135</v>
+      </c>
+      <c r="S15" s="73" t="s">
+        <v>169</v>
+      </c>
+      <c r="T15" s="74">
+        <v>11</v>
+      </c>
+      <c r="U15" s="74" t="s">
+        <v>171</v>
+      </c>
+      <c r="V15" s="74"/>
+      <c r="W15" s="73" t="s">
+        <v>174</v>
+      </c>
+      <c r="X15" s="73"/>
+    </row>
+    <row r="16" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B16" s="62" t="s">
+        <v>162</v>
+      </c>
+      <c r="J16" s="76" t="s">
+        <v>156</v>
+      </c>
+      <c r="K16" s="76" t="s">
+        <v>175</v>
+      </c>
+      <c r="L16" s="77">
+        <v>50</v>
+      </c>
+      <c r="M16" s="77" t="s">
+        <v>171</v>
+      </c>
+      <c r="N16" s="77"/>
+      <c r="O16" s="76" t="s">
+        <v>174</v>
+      </c>
+      <c r="P16" s="78"/>
+      <c r="R16" s="73" t="s">
+        <v>136</v>
+      </c>
+      <c r="S16" s="73" t="s">
+        <v>175</v>
+      </c>
+      <c r="T16" s="74">
+        <v>25</v>
+      </c>
+      <c r="U16" s="74" t="s">
+        <v>171</v>
+      </c>
+      <c r="V16" s="74"/>
+      <c r="W16" s="73" t="s">
+        <v>174</v>
+      </c>
+      <c r="X16" s="73"/>
+    </row>
+    <row r="17" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B17" s="63" t="s">
+        <v>163</v>
+      </c>
+      <c r="R17" s="73" t="s">
+        <v>137</v>
+      </c>
+      <c r="S17" s="73" t="s">
+        <v>175</v>
+      </c>
+      <c r="T17" s="74">
+        <v>25</v>
+      </c>
+      <c r="U17" s="74" t="s">
+        <v>171</v>
+      </c>
+      <c r="V17" s="74"/>
+      <c r="W17" s="73" t="s">
+        <v>174</v>
+      </c>
+      <c r="X17" s="73"/>
+    </row>
+    <row r="18" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="J18" s="64" t="s">
+        <v>176</v>
+      </c>
+      <c r="K18" s="65"/>
+      <c r="L18" s="66"/>
+      <c r="M18" s="66"/>
+      <c r="N18" s="66"/>
+      <c r="O18" s="65"/>
+      <c r="P18" s="67"/>
+      <c r="R18" s="73" t="s">
+        <v>119</v>
+      </c>
+      <c r="S18" s="73" t="s">
+        <v>175</v>
+      </c>
+      <c r="T18" s="74">
+        <v>50</v>
+      </c>
+      <c r="U18" s="74" t="s">
+        <v>171</v>
+      </c>
+      <c r="V18" s="74"/>
+      <c r="W18" s="73" t="s">
+        <v>174</v>
+      </c>
+      <c r="X18" s="73"/>
+    </row>
+    <row r="19" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="J19" s="58" t="s">
+        <v>164</v>
+      </c>
+      <c r="K19" s="58" t="s">
+        <v>102</v>
+      </c>
+      <c r="L19" s="58" t="s">
+        <v>170</v>
+      </c>
+      <c r="M19" s="58" t="s">
+        <v>165</v>
+      </c>
+      <c r="N19" s="58" t="s">
+        <v>166</v>
+      </c>
+      <c r="O19" s="68" t="s">
+        <v>167</v>
+      </c>
+      <c r="P19" s="69" t="s">
+        <v>168</v>
+      </c>
+      <c r="R19" s="73" t="s">
+        <v>120</v>
+      </c>
+      <c r="S19" s="73" t="s">
+        <v>175</v>
+      </c>
+      <c r="T19" s="74">
+        <v>50</v>
+      </c>
+      <c r="U19" s="74" t="s">
+        <v>171</v>
+      </c>
+      <c r="V19" s="74"/>
+      <c r="W19" s="73" t="s">
+        <v>174</v>
+      </c>
+      <c r="X19" s="73"/>
+    </row>
+    <row r="20" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="J20" s="70" t="s">
+        <v>115</v>
+      </c>
+      <c r="K20" s="70" t="s">
+        <v>169</v>
+      </c>
+      <c r="L20" s="71">
+        <v>5</v>
+      </c>
+      <c r="M20" s="71" t="s">
+        <v>171</v>
+      </c>
+      <c r="N20" s="71" t="s">
+        <v>172</v>
+      </c>
+      <c r="O20" s="70" t="s">
+        <v>174</v>
+      </c>
+      <c r="P20" s="72"/>
+      <c r="R20" s="73" t="s">
+        <v>127</v>
+      </c>
+      <c r="S20" s="73" t="s">
+        <v>175</v>
+      </c>
+      <c r="T20" s="74">
+        <v>25</v>
+      </c>
+      <c r="U20" s="74" t="s">
+        <v>171</v>
+      </c>
+      <c r="V20" s="74"/>
+      <c r="W20" s="73" t="s">
+        <v>174</v>
+      </c>
+      <c r="X20" s="73"/>
+    </row>
+    <row r="21" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="J21" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="K21" s="73" t="s">
+        <v>169</v>
+      </c>
+      <c r="L21" s="74">
+        <v>8</v>
+      </c>
+      <c r="M21" s="74" t="s">
+        <v>171</v>
+      </c>
+      <c r="N21" s="74" t="s">
+        <v>173</v>
+      </c>
+      <c r="O21" s="73" t="s">
+        <v>174</v>
+      </c>
+      <c r="P21" s="75"/>
+      <c r="R21" s="73" t="s">
+        <v>126</v>
+      </c>
+      <c r="S21" s="73" t="s">
+        <v>169</v>
+      </c>
+      <c r="T21" s="74">
+        <v>10</v>
+      </c>
+      <c r="U21" s="74" t="s">
+        <v>171</v>
+      </c>
+      <c r="V21" s="74" t="s">
+        <v>172</v>
+      </c>
+      <c r="W21" s="73" t="s">
+        <v>174</v>
+      </c>
+      <c r="X21" s="73"/>
+    </row>
+    <row r="22" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="J22" s="73" t="s">
+        <v>130</v>
+      </c>
+      <c r="K22" s="73" t="s">
+        <v>175</v>
+      </c>
+      <c r="L22" s="74">
+        <v>25</v>
+      </c>
+      <c r="M22" s="74" t="s">
+        <v>171</v>
+      </c>
+      <c r="N22" s="74"/>
+      <c r="O22" s="73" t="s">
+        <v>174</v>
+      </c>
+      <c r="P22" s="75"/>
+      <c r="R22" s="73" t="s">
+        <v>121</v>
+      </c>
+      <c r="S22" s="73" t="s">
+        <v>175</v>
+      </c>
+      <c r="T22" s="74">
+        <v>25</v>
+      </c>
+      <c r="U22" s="74" t="s">
+        <v>171</v>
+      </c>
+      <c r="V22" s="74"/>
+      <c r="W22" s="73" t="s">
+        <v>174</v>
+      </c>
+      <c r="X22" s="73"/>
+    </row>
+    <row r="23" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="J23" s="73" t="s">
+        <v>124</v>
+      </c>
+      <c r="K23" s="73" t="s">
+        <v>175</v>
+      </c>
+      <c r="L23" s="74">
+        <v>50</v>
+      </c>
+      <c r="M23" s="74" t="s">
+        <v>171</v>
+      </c>
+      <c r="N23" s="74"/>
+      <c r="O23" s="73" t="s">
+        <v>174</v>
+      </c>
+      <c r="P23" s="75"/>
+      <c r="R23" s="73" t="s">
+        <v>138</v>
+      </c>
+      <c r="S23" s="73" t="s">
+        <v>175</v>
+      </c>
+      <c r="T23" s="74">
+        <v>25</v>
+      </c>
+      <c r="U23" s="74" t="s">
+        <v>171</v>
+      </c>
+      <c r="V23" s="73"/>
+      <c r="W23" s="73"/>
+      <c r="X23" s="73"/>
+    </row>
+    <row r="24" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="J24" s="73" t="s">
+        <v>125</v>
+      </c>
+      <c r="K24" s="73" t="s">
+        <v>175</v>
+      </c>
+      <c r="L24" s="74">
+        <v>50</v>
+      </c>
+      <c r="M24" s="74" t="s">
+        <v>171</v>
+      </c>
+      <c r="N24" s="74"/>
+      <c r="O24" s="73" t="s">
+        <v>174</v>
+      </c>
+      <c r="P24" s="75"/>
+      <c r="R24" s="76" t="s">
+        <v>139</v>
+      </c>
+      <c r="S24" s="76" t="s">
+        <v>169</v>
+      </c>
+      <c r="T24" s="77">
+        <v>11</v>
+      </c>
+      <c r="U24" s="77" t="s">
+        <v>171</v>
+      </c>
+      <c r="V24" s="76"/>
+      <c r="W24" s="76"/>
+      <c r="X24" s="76"/>
+    </row>
+    <row r="25" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="J25" s="73" t="s">
+        <v>150</v>
+      </c>
+      <c r="K25" s="73" t="s">
+        <v>175</v>
+      </c>
+      <c r="L25" s="74">
+        <v>50</v>
+      </c>
+      <c r="M25" s="74" t="s">
+        <v>171</v>
+      </c>
+      <c r="N25" s="74"/>
+      <c r="O25" s="73" t="s">
+        <v>174</v>
+      </c>
+      <c r="P25" s="75"/>
+    </row>
+    <row r="26" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="J26" s="73" t="s">
+        <v>151</v>
+      </c>
+      <c r="K26" s="73" t="s">
+        <v>175</v>
+      </c>
+      <c r="L26" s="74">
+        <v>50</v>
+      </c>
+      <c r="M26" s="74" t="s">
+        <v>171</v>
+      </c>
+      <c r="N26" s="74"/>
+      <c r="O26" s="73" t="s">
+        <v>174</v>
+      </c>
+      <c r="P26" s="75"/>
+    </row>
+    <row r="27" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="J27" s="73" t="s">
+        <v>106</v>
+      </c>
+      <c r="K27" s="73" t="s">
+        <v>169</v>
+      </c>
+      <c r="L27" s="74">
+        <v>11</v>
+      </c>
+      <c r="M27" s="74" t="s">
+        <v>171</v>
+      </c>
+      <c r="N27" s="74"/>
+      <c r="O27" s="73" t="s">
+        <v>174</v>
+      </c>
+      <c r="P27" s="75"/>
+    </row>
+    <row r="28" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="J28" s="73" t="s">
+        <v>119</v>
+      </c>
+      <c r="K28" s="73" t="s">
+        <v>175</v>
+      </c>
+      <c r="L28" s="74">
+        <v>50</v>
+      </c>
+      <c r="M28" s="74" t="s">
+        <v>171</v>
+      </c>
+      <c r="N28" s="74"/>
+      <c r="O28" s="73" t="s">
+        <v>174</v>
+      </c>
+      <c r="P28" s="75"/>
+    </row>
+    <row r="29" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="J29" s="76" t="s">
+        <v>120</v>
+      </c>
+      <c r="K29" s="76" t="s">
+        <v>175</v>
+      </c>
+      <c r="L29" s="77">
+        <v>50</v>
+      </c>
+      <c r="M29" s="77" t="s">
+        <v>171</v>
+      </c>
+      <c r="N29" s="77"/>
+      <c r="O29" s="76" t="s">
+        <v>174</v>
+      </c>
+      <c r="P29" s="78"/>
+    </row>
+    <row r="32" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="J32" s="64" t="s">
+        <v>176</v>
+      </c>
+      <c r="K32" s="65"/>
+      <c r="L32" s="66"/>
+      <c r="M32" s="66"/>
+      <c r="N32" s="66"/>
+      <c r="O32" s="65"/>
+      <c r="P32" s="67"/>
+    </row>
+    <row r="33" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J33" s="58" t="s">
+        <v>164</v>
+      </c>
+      <c r="K33" s="58" t="s">
+        <v>102</v>
+      </c>
+      <c r="L33" s="58" t="s">
+        <v>170</v>
+      </c>
+      <c r="M33" s="58" t="s">
+        <v>165</v>
+      </c>
+      <c r="N33" s="58" t="s">
+        <v>166</v>
+      </c>
+      <c r="O33" s="68" t="s">
+        <v>167</v>
+      </c>
+      <c r="P33" s="69" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="34" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J34" s="70" t="s">
+        <v>115</v>
+      </c>
+      <c r="K34" s="70" t="s">
+        <v>169</v>
+      </c>
+      <c r="L34" s="71">
+        <v>5</v>
+      </c>
+      <c r="M34" s="71" t="s">
+        <v>171</v>
+      </c>
+      <c r="N34" s="71" t="s">
+        <v>173</v>
+      </c>
+      <c r="O34" s="70" t="s">
+        <v>174</v>
+      </c>
+      <c r="P34" s="72"/>
+    </row>
+    <row r="35" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J35" s="73" t="s">
+        <v>116</v>
+      </c>
+      <c r="K35" s="73" t="s">
+        <v>175</v>
+      </c>
+      <c r="L35" s="74">
+        <v>50</v>
+      </c>
+      <c r="M35" s="74" t="s">
+        <v>171</v>
+      </c>
+      <c r="N35" s="74"/>
+      <c r="O35" s="73" t="s">
+        <v>174</v>
+      </c>
+      <c r="P35" s="75"/>
+    </row>
+    <row r="36" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J36" s="73" t="s">
+        <v>117</v>
+      </c>
+      <c r="K36" s="73" t="s">
+        <v>175</v>
+      </c>
+      <c r="L36" s="74">
+        <v>50</v>
+      </c>
+      <c r="M36" s="74" t="s">
+        <v>171</v>
+      </c>
+      <c r="N36" s="74"/>
+      <c r="O36" s="73" t="s">
+        <v>174</v>
+      </c>
+      <c r="P36" s="75"/>
+    </row>
+    <row r="37" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J37" s="73" t="s">
+        <v>118</v>
+      </c>
+      <c r="K37" s="73" t="s">
+        <v>175</v>
+      </c>
+      <c r="L37" s="74">
+        <v>50</v>
+      </c>
+      <c r="M37" s="74" t="s">
+        <v>171</v>
+      </c>
+      <c r="N37" s="74"/>
+      <c r="O37" s="73" t="s">
+        <v>174</v>
+      </c>
+      <c r="P37" s="75"/>
+    </row>
+    <row r="38" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J38" s="73" t="s">
+        <v>154</v>
+      </c>
+      <c r="K38" s="73" t="s">
+        <v>175</v>
+      </c>
+      <c r="L38" s="74">
+        <v>10</v>
+      </c>
+      <c r="M38" s="74" t="s">
+        <v>171</v>
+      </c>
+      <c r="N38" s="74"/>
+      <c r="O38" s="73" t="s">
+        <v>174</v>
+      </c>
+      <c r="P38" s="75"/>
+    </row>
+    <row r="39" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J39" s="73" t="s">
+        <v>121</v>
+      </c>
+      <c r="K39" s="73" t="s">
+        <v>175</v>
+      </c>
+      <c r="L39" s="74">
+        <v>25</v>
+      </c>
+      <c r="M39" s="74" t="s">
+        <v>171</v>
+      </c>
+      <c r="N39" s="74"/>
+      <c r="O39" s="73" t="s">
+        <v>174</v>
+      </c>
+      <c r="P39" s="75"/>
+    </row>
+    <row r="40" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J40" s="73" t="s">
+        <v>132</v>
+      </c>
+      <c r="K40" s="73" t="s">
+        <v>175</v>
+      </c>
+      <c r="L40" s="74">
+        <v>5</v>
+      </c>
+      <c r="M40" s="74" t="s">
+        <v>171</v>
+      </c>
+      <c r="N40" s="74"/>
+      <c r="O40" s="73" t="s">
+        <v>174</v>
+      </c>
+      <c r="P40" s="75"/>
+    </row>
+    <row r="41" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J41" s="73" t="s">
+        <v>137</v>
+      </c>
+      <c r="K41" s="73" t="s">
+        <v>175</v>
+      </c>
+      <c r="L41" s="74">
+        <v>25</v>
+      </c>
+      <c r="M41" s="74" t="s">
+        <v>171</v>
+      </c>
+      <c r="N41" s="74"/>
+      <c r="O41" s="73" t="s">
+        <v>174</v>
+      </c>
+      <c r="P41" s="75"/>
+    </row>
+    <row r="42" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J42" s="76" t="s">
+        <v>122</v>
+      </c>
+      <c r="K42" s="76" t="s">
+        <v>175</v>
+      </c>
+      <c r="L42" s="77">
+        <v>3</v>
+      </c>
+      <c r="M42" s="77" t="s">
+        <v>171</v>
+      </c>
+      <c r="N42" s="77"/>
+      <c r="O42" s="76" t="s">
+        <v>174</v>
+      </c>
+      <c r="P42" s="78"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O74"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H10" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView showGridLines="0" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1344,8 +3004,8 @@
     <col min="4" max="4" width="5.21875" customWidth="1"/>
     <col min="5" max="5" width="24.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.109375" customWidth="1"/>
-    <col min="7" max="7" width="29" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.33203125" customWidth="1"/>
+    <col min="7" max="7" width="52.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.21875" customWidth="1"/>
     <col min="9" max="9" width="23.5546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7" style="7" customWidth="1"/>
     <col min="11" max="11" width="29" bestFit="1" customWidth="1"/>
@@ -1425,7 +3085,7 @@
         <v>19</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -1449,7 +3109,7 @@
       </c>
       <c r="K4" s="24"/>
       <c r="M4" s="6" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -1491,7 +3151,7 @@
       <c r="J6" s="42"/>
       <c r="K6" s="24"/>
       <c r="M6" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
@@ -1506,7 +3166,7 @@
       <c r="J7" s="42"/>
       <c r="K7" s="24"/>
       <c r="M7" s="6" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
@@ -1903,7 +3563,9 @@
         <v>142</v>
       </c>
       <c r="F36" s="21"/>
-      <c r="G36" s="24"/>
+      <c r="G36" s="24" t="s">
+        <v>190</v>
+      </c>
       <c r="I36" s="45" t="s">
         <v>102</v>
       </c>
@@ -1935,7 +3597,9 @@
         <v>143</v>
       </c>
       <c r="F38" s="21"/>
-      <c r="G38" s="24"/>
+      <c r="G38" s="24" t="s">
+        <v>189</v>
+      </c>
       <c r="I38" s="45" t="s">
         <v>100</v>
       </c>
@@ -1949,7 +3613,9 @@
         <v>144</v>
       </c>
       <c r="F39" s="21"/>
-      <c r="G39" s="24"/>
+      <c r="G39" s="83" t="s">
+        <v>188</v>
+      </c>
       <c r="I39" s="45" t="s">
         <v>99</v>
       </c>
@@ -1963,7 +3629,9 @@
         <v>156</v>
       </c>
       <c r="F40" s="21"/>
-      <c r="G40" s="24"/>
+      <c r="G40" s="57" t="s">
+        <v>197</v>
+      </c>
       <c r="I40" s="45" t="s">
         <v>101</v>
       </c>
@@ -1992,6 +3660,9 @@
       </c>
     </row>
     <row r="43" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="E43" t="s">
+        <v>191</v>
+      </c>
       <c r="I43" s="1" t="s">
         <v>79</v>
       </c>
@@ -2001,6 +3672,9 @@
       </c>
     </row>
     <row r="44" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="E44" t="s">
+        <v>192</v>
+      </c>
       <c r="I44" t="s">
         <v>0</v>
       </c>
@@ -2010,6 +3684,9 @@
       </c>
     </row>
     <row r="45" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="E45" t="s">
+        <v>193</v>
+      </c>
       <c r="I45" s="4" t="s">
         <v>36</v>
       </c>
@@ -2019,6 +3696,9 @@
       </c>
     </row>
     <row r="46" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="E46" t="s">
+        <v>194</v>
+      </c>
       <c r="I46" s="32" t="s">
         <v>85</v>
       </c>
@@ -2027,6 +3707,9 @@
       </c>
     </row>
     <row r="47" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="E47" t="s">
+        <v>195</v>
+      </c>
       <c r="I47" s="31" t="s">
         <v>86</v>
       </c>
@@ -2035,6 +3718,9 @@
       </c>
     </row>
     <row r="48" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="E48" t="s">
+        <v>196</v>
+      </c>
       <c r="I48" s="8" t="s">
         <v>39</v>
       </c>
@@ -2043,7 +3729,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="49" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="49" spans="5:15" x14ac:dyDescent="0.3">
       <c r="F49" s="1"/>
       <c r="I49" s="8" t="s">
         <v>37</v>
@@ -2053,7 +3739,10 @@
         <v>73</v>
       </c>
     </row>
-    <row r="50" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="50" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="E50" t="s">
+        <v>199</v>
+      </c>
       <c r="I50" s="8" t="s">
         <v>42</v>
       </c>
@@ -2062,7 +3751,10 @@
         <v>40</v>
       </c>
     </row>
-    <row r="51" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="51" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="E51" t="s">
+        <v>198</v>
+      </c>
       <c r="F51" s="4"/>
       <c r="I51" s="8" t="s">
         <v>43</v>
@@ -2072,17 +3764,17 @@
         <v>41</v>
       </c>
     </row>
-    <row r="52" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="52" spans="5:15" x14ac:dyDescent="0.3">
       <c r="I52" s="8" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="53" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="53" spans="5:15" x14ac:dyDescent="0.3">
       <c r="I53" s="8" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="54" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="54" spans="5:15" x14ac:dyDescent="0.3">
       <c r="I54" s="8" t="s">
         <v>84</v>
       </c>
@@ -2090,13 +3782,13 @@
         <v>114</v>
       </c>
     </row>
-    <row r="55" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="55" spans="5:15" x14ac:dyDescent="0.3">
       <c r="I55" s="8" t="s">
         <v>40</v>
       </c>
       <c r="J55" s="46"/>
     </row>
-    <row r="56" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="56" spans="5:15" x14ac:dyDescent="0.3">
       <c r="I56" s="8" t="s">
         <v>41</v>
       </c>
@@ -2109,7 +3801,7 @@
       </c>
       <c r="O56" s="51"/>
     </row>
-    <row r="57" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="57" spans="5:15" x14ac:dyDescent="0.3">
       <c r="I57" s="8" t="s">
         <v>38</v>
       </c>
@@ -2126,7 +3818,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="58" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="58" spans="5:15" x14ac:dyDescent="0.3">
       <c r="I58" s="8" t="s">
         <v>35</v>
       </c>
@@ -2141,7 +3833,7 @@
       </c>
       <c r="O58" s="8"/>
     </row>
-    <row r="59" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="59" spans="5:15" x14ac:dyDescent="0.3">
       <c r="I59" s="8"/>
       <c r="M59" s="8" t="s">
         <v>5</v>
@@ -2149,14 +3841,14 @@
       <c r="N59" s="42"/>
       <c r="O59" s="8"/>
     </row>
-    <row r="60" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="60" spans="5:15" x14ac:dyDescent="0.3">
       <c r="M60" s="8" t="s">
         <v>10</v>
       </c>
       <c r="N60" s="42"/>
       <c r="O60" s="8"/>
     </row>
-    <row r="61" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="61" spans="5:15" x14ac:dyDescent="0.3">
       <c r="I61" s="34" t="s">
         <v>76</v>
       </c>
@@ -2168,7 +3860,7 @@
       <c r="N61" s="42"/>
       <c r="O61" s="8"/>
     </row>
-    <row r="62" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="62" spans="5:15" x14ac:dyDescent="0.3">
       <c r="I62" s="35" t="s">
         <v>85</v>
       </c>
@@ -2180,7 +3872,7 @@
       <c r="N62" s="42"/>
       <c r="O62" s="8"/>
     </row>
-    <row r="63" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="63" spans="5:15" x14ac:dyDescent="0.3">
       <c r="I63" s="36" t="s">
         <v>86</v>
       </c>
@@ -2194,7 +3886,7 @@
       <c r="N63" s="42"/>
       <c r="O63" s="8"/>
     </row>
-    <row r="64" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="64" spans="5:15" x14ac:dyDescent="0.3">
       <c r="I64" s="10" t="s">
         <v>39</v>
       </c>
@@ -2319,18 +4011,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="28.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -2434,6 +4127,11 @@
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>87</v>
+      </c>
+    </row>
+    <row r="59" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C59">
+        <v>5497844651</v>
       </c>
     </row>
   </sheetData>
@@ -2442,12 +4140,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:C13"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2562,16 +4260,171 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:F37"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView showGridLines="0" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="P43" sqref="P43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="1.21875" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="0.88671875" customWidth="1"/>
+    <col min="5" max="5" width="20.88671875" customWidth="1"/>
+    <col min="6" max="6" width="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" ht="20.399999999999999" x14ac:dyDescent="0.45">
+      <c r="B2" s="81"/>
+      <c r="C2" s="82" t="s">
+        <v>187</v>
+      </c>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B3" s="79"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B4" s="79"/>
+      <c r="C4" s="79" t="s">
+        <v>183</v>
+      </c>
+      <c r="D4" s="79"/>
+      <c r="E4" s="84" t="s">
+        <v>185</v>
+      </c>
+      <c r="F4" s="79"/>
+    </row>
+    <row r="5" spans="2:6" ht="3.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="79"/>
+      <c r="C5" s="79"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="80"/>
+      <c r="F5" s="79"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B6" s="79"/>
+      <c r="C6" s="79" t="s">
+        <v>184</v>
+      </c>
+      <c r="D6" s="79"/>
+      <c r="E6" s="84" t="s">
+        <v>186</v>
+      </c>
+      <c r="F6" s="79"/>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B7" s="79"/>
+      <c r="C7" s="79"/>
+      <c r="D7" s="79"/>
+      <c r="E7" s="79"/>
+      <c r="F7" s="79"/>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B8" s="79"/>
+      <c r="C8" s="79"/>
+      <c r="D8" s="79"/>
+      <c r="E8" s="79"/>
+      <c r="F8" s="79"/>
+    </row>
+    <row r="9" spans="2:6" ht="7.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="79"/>
+      <c r="C9" s="79"/>
+      <c r="D9" s="79"/>
+      <c r="E9" s="79"/>
+      <c r="F9" s="79"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="29" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C29" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="30" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C30" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="31" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C31" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="32" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C32" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C33" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C34" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C35" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C36" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C37" t="s">
+        <v>202</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
5th day planning, datamapping, schema, login page and 4 Classes
</commit_message>
<xml_diff>
--- a/ToniProject.xlsx
+++ b/ToniProject.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Schema" sheetId="6" r:id="rId1"/>
@@ -876,7 +876,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -934,6 +934,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1088,7 +1094,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1214,6 +1220,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1507,10 +1514,10 @@
       <xdr:rowOff>22861</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>182880</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>3351</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>403860</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>75888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1528,7 +1535,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="224525" y="3345181"/>
-          <a:ext cx="9750055" cy="1077770"/>
+          <a:ext cx="8751835" cy="967427"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1540,15 +1547,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>45721</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
+      <xdr:rowOff>121920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>4466</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>98574</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>255047</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1565,8 +1572,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="5646420"/>
-          <a:ext cx="13453766" cy="2895114"/>
+          <a:off x="45721" y="6918960"/>
+          <a:ext cx="8781826" cy="1889760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1843,8 +1850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:X42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView showGridLines="0" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -2777,7 +2784,7 @@
     </row>
     <row r="32" spans="2:24" x14ac:dyDescent="0.3">
       <c r="J32" s="64" t="s">
-        <v>176</v>
+        <v>146</v>
       </c>
       <c r="K32" s="65"/>
       <c r="L32" s="66"/>
@@ -2992,8 +2999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O74"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M26" sqref="M26:M53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4016,7 +4023,7 @@
   <dimension ref="A1:C59"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="A8" sqref="A8:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4262,10 +4269,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F37"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="P43" sqref="P43"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4277,7 +4284,17 @@
     <col min="6" max="6" width="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="20.399999999999999" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="85"/>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+    </row>
+    <row r="2" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.45">
+      <c r="A2" s="85"/>
       <c r="B2" s="81"/>
       <c r="C2" s="82" t="s">
         <v>187</v>
@@ -4285,15 +4302,19 @@
       <c r="D2" s="81"/>
       <c r="E2" s="81"/>
       <c r="F2" s="81"/>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G2" s="85"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="85"/>
       <c r="B3" s="79"/>
       <c r="C3" s="79"/>
       <c r="D3" s="79"/>
       <c r="E3" s="79"/>
       <c r="F3" s="79"/>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G3" s="85"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="85"/>
       <c r="B4" s="79"/>
       <c r="C4" s="79" t="s">
         <v>183</v>
@@ -4303,15 +4324,19 @@
         <v>185</v>
       </c>
       <c r="F4" s="79"/>
-    </row>
-    <row r="5" spans="2:6" ht="3.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G4" s="85"/>
+    </row>
+    <row r="5" spans="1:7" ht="3.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="85"/>
       <c r="B5" s="79"/>
       <c r="C5" s="79"/>
       <c r="D5" s="79"/>
       <c r="E5" s="80"/>
       <c r="F5" s="79"/>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G5" s="85"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="85"/>
       <c r="B6" s="79"/>
       <c r="C6" s="79" t="s">
         <v>184</v>
@@ -4321,49 +4346,65 @@
         <v>186</v>
       </c>
       <c r="F6" s="79"/>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G6" s="85"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="85"/>
       <c r="B7" s="79"/>
       <c r="C7" s="79"/>
       <c r="D7" s="79"/>
       <c r="E7" s="79"/>
       <c r="F7" s="79"/>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G7" s="85"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="85"/>
       <c r="B8" s="79"/>
       <c r="C8" s="79"/>
       <c r="D8" s="79"/>
       <c r="E8" s="79"/>
       <c r="F8" s="79"/>
-    </row>
-    <row r="9" spans="2:6" ht="7.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G8" s="85"/>
+    </row>
+    <row r="9" spans="1:7" ht="7.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="85"/>
       <c r="B9" s="79"/>
       <c r="C9" s="79"/>
       <c r="D9" s="79"/>
       <c r="E9" s="79"/>
       <c r="F9" s="79"/>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G9" s="85"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="85"/>
+      <c r="B10" s="85"/>
+      <c r="C10" s="85"/>
+      <c r="D10" s="85"/>
+      <c r="E10" s="85"/>
+      <c r="F10" s="85"/>
+      <c r="G10" s="85"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
         <v>212</v>
       </c>

</xml_diff>